<commit_message>
Updated BOM items yet to arrive  file
</commit_message>
<xml_diff>
--- a/ProjectHugo_BOM_Items_yet_to_Arrive.xlsx
+++ b/ProjectHugo_BOM_Items_yet_to_Arrive.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -95,20 +95,6 @@
   </si>
   <si>
     <t>https://www.amazon.de/-/en/KeeYees-120pcs-Jumper-Arduino-Raspberry/dp/B07KCD7GS7/ref=sr_1_3?dchild=1&amp;keywords=male+header&amp;qid=1608576987&amp;s=ce-de&amp;sr=1-3</t>
-  </si>
-  <si>
-    <t>B00IYUWT2A</t>
-  </si>
-  <si>
-    <t>Resistors</t>
-  </si>
-  <si>
-    <t>10 KOhm for the sensor design
-30x Resistors pack 
-(in total 32 peices)</t>
-  </si>
-  <si>
-    <t>https://www.amazon.de/Widerstand-St%C3%BCck-Kohleschicht-Widerst%C3%A4nde-Resistor/dp/B00IYUWT2A/ref=sr_1_8?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crresistor+10kohmd=3MG66TQKIM9KI&amp;dchild=1&amp;keywords=resistor+10k+ohm&amp;qid=1607692043&amp;sprefix=resistor+%2Caps%2C183&amp;sr=8-8</t>
   </si>
   <si>
     <t>Total</t>
@@ -206,11 +192,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$€]#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$€]#,##0.00"/>
   </numFmts>
   <fonts count="42">
     <font>
@@ -357,8 +343,17 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,6 +373,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -385,9 +388,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,23 +397,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -466,7 +459,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -479,6 +479,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -487,22 +488,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -565,13 +551,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,19 +599,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,7 +623,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,7 +677,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,31 +695,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,79 +731,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -833,17 +819,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -889,24 +884,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -919,162 +916,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1110,7 +1096,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1243,40 +1229,40 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="15" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="19" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="20" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="20" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="7" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="15" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="19" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="19" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="12" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1444,14 +1430,14 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1685925" cy="1476375"/>
+    <xdr:ext cx="2238375" cy="1952625"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="image7.jpg"/>
+        <xdr:cNvPr id="13" name="image1.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1462,39 +1448,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7319010" y="5686425"/>
-          <a:ext cx="1685925" cy="1476375"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2238375" cy="1952625"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="image1.jpg"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId5" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7067550" y="8524875"/>
+          <a:off x="7067550" y="7048500"/>
           <a:ext cx="2238375" cy="1952625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1509,7 +1463,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>1935480</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1771650" cy="1152525"/>
@@ -1519,14 +1473,14 @@
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId6" cstate="print"/>
+        <a:blip r:embed="rId5" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7372350" y="10460355"/>
+          <a:off x="7372350" y="8983980"/>
           <a:ext cx="1771650" cy="1152525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1541,7 +1495,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1057275" cy="1057275"/>
@@ -1551,14 +1505,14 @@
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7" cstate="print"/>
+        <a:blip r:embed="rId6" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7715250" y="11652885"/>
+          <a:off x="7715250" y="10176510"/>
           <a:ext cx="1057275" cy="1057275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1573,13 +1527,45 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>632460</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1043940</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="581025" cy="1752600"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="18" name="image13.jpg"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7700010" y="11197590"/>
+          <a:ext cx="581025" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1762125" cy="1104900"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="image5.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1590,8 +1576,40 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7700010" y="12673965"/>
-          <a:ext cx="581025" cy="1752600"/>
+          <a:off x="7067550" y="12963525"/>
+          <a:ext cx="1762125" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1895475" cy="1866900"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="image19.jpg"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7067550" y="12963525"/>
+          <a:ext cx="1895475" cy="1866900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1608,22 +1626,22 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1762125" cy="1104900"/>
+    <xdr:ext cx="1095375" cy="914400"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="image5.jpg"/>
+        <xdr:cNvPr id="22" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9" cstate="print"/>
+        <a:blip r:embed="rId10" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7067550" y="14439900"/>
-          <a:ext cx="1762125" cy="1104900"/>
+          <a:off x="7067550" y="14830425"/>
+          <a:ext cx="1095375" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1640,42 +1658,10 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1895475" cy="1866900"/>
+    <xdr:ext cx="1409700" cy="1219200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="image19.jpg"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId10" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7067550" y="14439900"/>
-          <a:ext cx="1895475" cy="1866900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1095375" cy="914400"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="image2.jpg"/>
+        <xdr:cNvPr id="25" name="image9.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1686,39 +1672,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7067550" y="16306800"/>
-          <a:ext cx="1095375" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1409700" cy="1219200"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="image9.jpg"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId12" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7067550" y="16306800"/>
+          <a:off x="7067550" y="14830425"/>
           <a:ext cx="1409700" cy="1219200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1933,12 +1887,12 @@
     <tabColor rgb="FF44546A"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="$A8:$XFD8"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="$A9:$XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1777777777778" defaultRowHeight="15" customHeight="1"/>
@@ -2021,8 +1975,8 @@
         <v>4</v>
       </c>
       <c r="C3" s="9">
-        <f>F19</f>
-        <v>11</v>
+        <f>F18</f>
+        <v>9</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="6"/>
@@ -2054,8 +2008,8 @@
         <v>5</v>
       </c>
       <c r="C4" s="11">
-        <f>J19</f>
-        <v>154.94</v>
+        <f>J18</f>
+        <v>148.64</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="6"/>
@@ -2245,33 +2199,21 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" ht="116.25" customHeight="1" spans="1:26">
-      <c r="A9" s="1"/>
-      <c r="B9" s="16" t="s">
+    <row r="9" ht="39.75" customHeight="1" spans="1:26">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17">
-        <v>2</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="56">
-        <v>3.15</v>
-      </c>
-      <c r="J9" s="57">
-        <f>F9*I9</f>
-        <v>6.3</v>
+      <c r="J9" s="60">
+        <f>SUM(J7:J8)</f>
+        <v>48</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -2290,72 +2232,84 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" ht="39.75" customHeight="1" spans="1:26">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="59" t="s">
+    <row r="10" ht="67.5" customHeight="1" spans="1:26">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
+      <c r="V10" s="63"/>
+      <c r="W10" s="63"/>
+      <c r="X10" s="63"/>
+      <c r="Y10" s="63"/>
+      <c r="Z10" s="63"/>
+    </row>
+    <row r="11" ht="153.75" customHeight="1" spans="1:26">
+      <c r="A11" s="1"/>
+      <c r="B11" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="60">
-        <f>SUM(J7:J9)</f>
-        <v>54.3</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-    </row>
-    <row r="11" ht="67.5" customHeight="1" spans="1:26">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="16"/>
+      <c r="F11" s="17">
+        <v>4</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
-      <c r="N11" s="63"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="63"/>
-      <c r="T11" s="63"/>
-      <c r="U11" s="63"/>
-      <c r="V11" s="63"/>
-      <c r="W11" s="63"/>
-      <c r="X11" s="63"/>
-      <c r="Y11" s="63"/>
-      <c r="Z11" s="63"/>
-    </row>
-    <row r="12" ht="153.75" customHeight="1" spans="1:26">
+      <c r="I11" s="56">
+        <v>8.71</v>
+      </c>
+      <c r="J11" s="57">
+        <f t="shared" ref="J11:J16" si="0">F11*I11</f>
+        <v>34.84</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+    </row>
+    <row r="12" ht="90.75" customHeight="1" spans="1:26">
       <c r="A12" s="1"/>
       <c r="B12" s="16" t="s">
         <v>31</v>
@@ -2368,20 +2322,20 @@
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="22" t="s">
         <v>18</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>34</v>
       </c>
       <c r="I12" s="56">
-        <v>8.71</v>
+        <v>32</v>
       </c>
       <c r="J12" s="57">
-        <f t="shared" ref="J12:J17" si="0">F12*I12</f>
-        <v>34.84</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -2400,7 +2354,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" ht="90.75" customHeight="1" spans="1:26">
+    <row r="13" ht="83.25" customHeight="1" spans="1:26">
       <c r="A13" s="1"/>
       <c r="B13" s="16" t="s">
         <v>35</v>
@@ -2415,18 +2369,18 @@
       <c r="F13" s="17">
         <v>1</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H13" s="19" t="s">
         <v>38</v>
       </c>
       <c r="I13" s="56">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="J13" s="57">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -2445,7 +2399,7 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" ht="83.25" customHeight="1" spans="1:26">
+    <row r="14" ht="138" customHeight="1" spans="1:26">
       <c r="A14" s="1"/>
       <c r="B14" s="16" t="s">
         <v>39</v>
@@ -2467,11 +2421,11 @@
         <v>42</v>
       </c>
       <c r="I14" s="56">
-        <v>16</v>
+        <v>9.9</v>
       </c>
       <c r="J14" s="57">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>9.9</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -2490,7 +2444,7 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" ht="138" customHeight="1" spans="1:26">
+    <row r="15" ht="147" customHeight="1" spans="1:26">
       <c r="A15" s="1"/>
       <c r="B15" s="16" t="s">
         <v>43</v>
@@ -2512,11 +2466,11 @@
         <v>46</v>
       </c>
       <c r="I15" s="56">
-        <v>9.9</v>
+        <v>6</v>
       </c>
       <c r="J15" s="57">
         <f t="shared" si="0"/>
-        <v>9.9</v>
+        <v>6</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2535,33 +2489,33 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" ht="147" customHeight="1" spans="1:26">
+    <row r="16" ht="96" customHeight="1" spans="1:26">
       <c r="A16" s="1"/>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17">
+      <c r="E16" s="34"/>
+      <c r="F16" s="35">
         <v>1</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="56">
-        <v>6</v>
+      <c r="I16" s="58">
+        <v>1.9</v>
       </c>
       <c r="J16" s="57">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1.9</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2580,33 +2534,21 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" ht="96" customHeight="1" spans="1:26">
+    <row r="17" ht="37.5" customHeight="1" spans="1:26">
       <c r="A17" s="1"/>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35">
-        <v>1</v>
-      </c>
-      <c r="G17" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="58">
-        <v>1.9</v>
-      </c>
-      <c r="J17" s="57">
-        <f t="shared" si="0"/>
-        <v>1.9</v>
+      <c r="J17" s="65">
+        <f>SUM(J11:J16)</f>
+        <v>100.64</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -2625,21 +2567,26 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" ht="37.5" customHeight="1" spans="1:26">
+    <row r="18" ht="39.75" customHeight="1" spans="1:26">
       <c r="A18" s="1"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="64" t="s">
-        <v>55</v>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45" t="s">
+        <v>52</v>
       </c>
-      <c r="J18" s="65">
-        <f>SUM(J12:J17)</f>
-        <v>100.64</v>
+      <c r="F18" s="46">
+        <f>SUM(F7:F12)</f>
+        <v>9</v>
+      </c>
+      <c r="G18" s="47"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="67">
+        <f>SUM(J9,J17)</f>
+        <v>148.64</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -2658,27 +2605,17 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" ht="39.75" customHeight="1" spans="1:26">
+    <row r="19" ht="15.75" customHeight="1" spans="1:26">
       <c r="A19" s="1"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="46">
-        <f>SUM(F7:F13)</f>
-        <v>11</v>
-      </c>
-      <c r="G19" s="47"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="J19" s="67">
-        <f>SUM(J10,J18)</f>
-        <v>154.94</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -2698,15 +2635,15 @@
     </row>
     <row r="20" ht="15.75" customHeight="1" spans="1:26">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="68"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -2726,15 +2663,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1" spans="1:26">
       <c r="A21" s="1"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
+      <c r="B21" s="51"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -2774,7 +2703,15 @@
     </row>
     <row r="23" ht="15.75" customHeight="1" spans="1:26">
       <c r="A23" s="1"/>
-      <c r="B23" s="51"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="68"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -30092,52 +30029,23 @@
       <c r="Y998" s="1"/>
       <c r="Z998" s="1"/>
     </row>
-    <row r="999" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A999" s="1"/>
-      <c r="B999" s="1"/>
-      <c r="C999" s="1"/>
-      <c r="D999" s="1"/>
-      <c r="E999" s="1"/>
-      <c r="F999" s="1"/>
-      <c r="G999" s="49"/>
-      <c r="H999" s="1"/>
-      <c r="I999" s="1"/>
-      <c r="J999" s="68"/>
-      <c r="K999" s="1"/>
-      <c r="L999" s="1"/>
-      <c r="M999" s="1"/>
-      <c r="N999" s="1"/>
-      <c r="O999" s="1"/>
-      <c r="P999" s="1"/>
-      <c r="Q999" s="1"/>
-      <c r="R999" s="1"/>
-      <c r="S999" s="1"/>
-      <c r="T999" s="1"/>
-      <c r="U999" s="1"/>
-      <c r="V999" s="1"/>
-      <c r="W999" s="1"/>
-      <c r="X999" s="1"/>
-      <c r="Y999" s="1"/>
-      <c r="Z999" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B21:J23"/>
+    <mergeCell ref="B20:J22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId2" display="https://www.amazon.de/-/en/Wingo-Engineer-Baite-02/dp/B01N2N7LZA/ref=sr_1_3?dchild=1&amp;keywords=Arduino%2BMega%2BShield&amp;qid=1608575610&amp;quartzVehicle=1480-1518&amp;replacementKeywords=arduino%2Bshield&amp;sr=8-3&amp;th=1"/>
     <hyperlink ref="H8" r:id="rId3" display="https://www.amazon.de/-/en/KeeYees-120pcs-Jumper-Arduino-Raspberry/dp/B07KCD7GS7/ref=sr_1_3?dchild=1&amp;keywords=male+header&amp;qid=1608576987&amp;s=ce-de&amp;sr=1-3"/>
-    <hyperlink ref="H9" r:id="rId4" display="https://www.amazon.de/Widerstand-St%C3%BCck-Kohleschicht-Widerst%C3%A4nde-Resistor/dp/B00IYUWT2A/ref=sr_1_8?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crresistor+10kohmd=3MG66TQKIM9KI&amp;dchild=1&amp;keywords=resistor+10k+ohm&amp;qid=1607692043&amp;sprefix=resistor+%2Caps%2C183&amp;sr=8-8"/>
-    <hyperlink ref="H12" r:id="rId5" display="https://www.amazon.de/ILS-Micro-1-5mm-Connector-Cables/dp/B07GXN2521/ref=sr_1_4?dchild=1&amp;keywords=jst+connector+6+pin&amp;qid=1607796071&amp;sr=8-4"/>
-    <hyperlink ref="H13" r:id="rId6" display="https://www.amazon.de/Supply-Netzteil-WS2801-WS2812-WS2812B/dp/B00KKVJ1H2"/>
-    <hyperlink ref="H14" r:id="rId7" display="https://www.amazon.de/dp/B08BR2CQRX/ref=sspa_dk_detail_9?psc=1&amp;pd_rd_i=B08BR2CQRX&amp;pd_rd_w=xh1zB&amp;pf_rd_p=403c666b-0b30-4f66-afde-0388ffdf2c39&amp;pd_rd_wg=BMAaq&amp;pf_rd_r=9V6R19D300YNTEH8X64R&amp;pd_rd_r=a3a85a8b-9567-402c-8027-6c74a513e3dd&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzQVBHTVU4VE03UklZJmVuY3J5cHRlZElkPUEwOTY1MTQxMVUyS0NCSkIxNFI4RSZlbmNyeXB0ZWRBZElkPUEwMTY3OTAyMUJDQUxZMDlTTDVQRiZ3aWRnZXROYW1lPXNwX2RldGFpbCZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU="/>
-    <hyperlink ref="H15" r:id="rId8" display="https://www.amazon.de/-/en/S-PolyBond%C2%AE-Acrylic-plexiglass-adhesive-suitable/dp/B07PNYJDZ7/ref=sr_1_6?crid=2TYVNVUVXCMGB&amp;dchild=1&amp;keywords=acrylkleber&amp;qid=1608107542&amp;sprefix=acrzlic+%2Caps%2C210&amp;sr=8-6"/>
-    <hyperlink ref="H16" r:id="rId9" display="https://www.amazon.de/dp/B07Y1TJH5R/ref=sspa_dk_detail_3?pd_rd_i=B07Y1T2LYG&amp;pd_rd_w=bOi2a&amp;pf_rd_p=907efdef-64f0-4d54-bac1-a1aa35942c8f&amp;pd_rd_wg=ftywR&amp;pf_rd_r=SNRDG5G2PHWXYMKK2S1Z&amp;pd_rd_r=c73f883a-8f8b-40d3-9ec3-bed71a77e59e&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUFGSUVDQlVVMkFZNjEmZW5jcnlwdGVkSWQ9QTA3ODU2NjgxQTFBUk1IWVA4N0hBJmVuY3J5cHRlZEFkSWQ9QTA5NjYzMDg4UTVKVU5EUlUwREgmd2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWMmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl&amp;th=1"/>
-    <hyperlink ref="H17" r:id="rId10" display="https://www.amazon.de/-/en/Aurora-trading-Shrink-Tubing-Choose-colours/dp/B00XZ7IEAS/ref=sr_1_27?dchild=1&amp;keywords=schrumpfschlauch&amp;qid=1608577108&amp;sr=8-27&amp;th=1"/>
+    <hyperlink ref="H11" r:id="rId4" display="https://www.amazon.de/ILS-Micro-1-5mm-Connector-Cables/dp/B07GXN2521/ref=sr_1_4?dchild=1&amp;keywords=jst+connector+6+pin&amp;qid=1607796071&amp;sr=8-4"/>
+    <hyperlink ref="H12" r:id="rId5" display="https://www.amazon.de/Supply-Netzteil-WS2801-WS2812-WS2812B/dp/B00KKVJ1H2"/>
+    <hyperlink ref="H13" r:id="rId6" display="https://www.amazon.de/dp/B08BR2CQRX/ref=sspa_dk_detail_9?psc=1&amp;pd_rd_i=B08BR2CQRX&amp;pd_rd_w=xh1zB&amp;pf_rd_p=403c666b-0b30-4f66-afde-0388ffdf2c39&amp;pd_rd_wg=BMAaq&amp;pf_rd_r=9V6R19D300YNTEH8X64R&amp;pd_rd_r=a3a85a8b-9567-402c-8027-6c74a513e3dd&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzQVBHTVU4VE03UklZJmVuY3J5cHRlZElkPUEwOTY1MTQxMVUyS0NCSkIxNFI4RSZlbmNyeXB0ZWRBZElkPUEwMTY3OTAyMUJDQUxZMDlTTDVQRiZ3aWRnZXROYW1lPXNwX2RldGFpbCZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU="/>
+    <hyperlink ref="H14" r:id="rId7" display="https://www.amazon.de/-/en/S-PolyBond%C2%AE-Acrylic-plexiglass-adhesive-suitable/dp/B07PNYJDZ7/ref=sr_1_6?crid=2TYVNVUVXCMGB&amp;dchild=1&amp;keywords=acrylkleber&amp;qid=1608107542&amp;sprefix=acrzlic+%2Caps%2C210&amp;sr=8-6"/>
+    <hyperlink ref="H15" r:id="rId8" display="https://www.amazon.de/dp/B07Y1TJH5R/ref=sspa_dk_detail_3?pd_rd_i=B07Y1T2LYG&amp;pd_rd_w=bOi2a&amp;pf_rd_p=907efdef-64f0-4d54-bac1-a1aa35942c8f&amp;pd_rd_wg=ftywR&amp;pf_rd_r=SNRDG5G2PHWXYMKK2S1Z&amp;pd_rd_r=c73f883a-8f8b-40d3-9ec3-bed71a77e59e&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUFGSUVDQlVVMkFZNjEmZW5jcnlwdGVkSWQ9QTA3ODU2NjgxQTFBUk1IWVA4N0hBJmVuY3J5cHRlZEFkSWQ9QTA5NjYzMDg4UTVKVU5EUlUwREgmd2lkZ2V0TmFtZT1zcF9kZXRhaWxfdGhlbWF0aWMmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl&amp;th=1"/>
+    <hyperlink ref="H16" r:id="rId9" display="https://www.amazon.de/-/en/Aurora-trading-Shrink-Tubing-Choose-colours/dp/B00XZ7IEAS/ref=sr_1_27?dchild=1&amp;keywords=schrumpfschlauch&amp;qid=1608577108&amp;sr=8-27&amp;th=1"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
+  <pageSetup paperSize="9" scale="33" fitToHeight="0" orientation="landscape"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>